<commit_message>
Add missing cities to dictionary
</commit_message>
<xml_diff>
--- a/Data dict - cities_with_city_id.xlsx
+++ b/Data dict - cities_with_city_id.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwoom\Documents\Airline Reviews Data Cleaning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C79A774-517E-4F28-8267-8836C899BDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B081F9C0-C497-44D5-877B-84716D163A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8051CC61-5052-4A8C-9131-2F5D376E408A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$3564</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$3562</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9541" uniqueCount="3810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9559" uniqueCount="3819">
   <si>
     <t>Aalborg</t>
   </si>
@@ -11470,6 +11470,33 @@
   </si>
   <si>
     <t>Toluca</t>
+  </si>
+  <si>
+    <t>Terceira</t>
+  </si>
+  <si>
+    <t>Southend</t>
+  </si>
+  <si>
+    <t>Salalah</t>
+  </si>
+  <si>
+    <t>Mahon</t>
+  </si>
+  <si>
+    <t>Lublin</t>
+  </si>
+  <si>
+    <t>Raipur</t>
+  </si>
+  <si>
+    <t>Pretoria</t>
+  </si>
+  <si>
+    <t>Tuzla</t>
+  </si>
+  <si>
+    <t>Ko Samui</t>
   </si>
 </sst>
 </file>
@@ -11842,10 +11869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E001419E-E630-4900-9D2F-B82230F85771}">
-  <dimension ref="A1:E3469"/>
+  <dimension ref="A1:E3478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3055" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3067" sqref="D3067"/>
+    <sheetView tabSelected="1" topLeftCell="A3464" zoomScale="113" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3470" sqref="F3470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57055,8 +57082,107 @@
         <v>3474</v>
       </c>
     </row>
+    <row r="3470" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3470" t="s">
+        <v>3810</v>
+      </c>
+      <c r="D3470" t="s">
+        <v>869</v>
+      </c>
+      <c r="E3470">
+        <v>3475</v>
+      </c>
+    </row>
+    <row r="3471" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3471" t="s">
+        <v>3811</v>
+      </c>
+      <c r="D3471" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3471">
+        <v>3476</v>
+      </c>
+    </row>
+    <row r="3472" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3472" t="s">
+        <v>3812</v>
+      </c>
+      <c r="D3472" t="s">
+        <v>2257</v>
+      </c>
+      <c r="E3472">
+        <v>3477</v>
+      </c>
+    </row>
+    <row r="3473" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3473" t="s">
+        <v>3813</v>
+      </c>
+      <c r="D3473" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3473">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="3474" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3474" t="s">
+        <v>3818</v>
+      </c>
+      <c r="D3474" t="s">
+        <v>341</v>
+      </c>
+      <c r="E3474">
+        <v>3479</v>
+      </c>
+    </row>
+    <row r="3475" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3475" t="s">
+        <v>3814</v>
+      </c>
+      <c r="D3475" t="s">
+        <v>633</v>
+      </c>
+      <c r="E3475">
+        <v>3480</v>
+      </c>
+    </row>
+    <row r="3476" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3476" t="s">
+        <v>3815</v>
+      </c>
+      <c r="D3476" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3476">
+        <v>3481</v>
+      </c>
+    </row>
+    <row r="3477" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3477" t="s">
+        <v>3816</v>
+      </c>
+      <c r="D3477" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3477">
+        <v>3482</v>
+      </c>
+    </row>
+    <row r="3478" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3478" t="s">
+        <v>3817</v>
+      </c>
+      <c r="D3478" t="s">
+        <v>2223</v>
+      </c>
+      <c r="E3478">
+        <v>3483</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:D3564" xr:uid="{E001419E-E630-4900-9D2F-B82230F85771}"/>
+  <autoFilter ref="A1:D3562" xr:uid="{E001419E-E630-4900-9D2F-B82230F85771}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>